<commit_message>
add real time notification
</commit_message>
<xml_diff>
--- a/uploads/rbt/excel/new/1508228742_rbtNew (2).xlsx
+++ b/uploads/rbt/excel/new/1508228742_rbtNew (2).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abubakr.sokarno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\rbt_system_php7\uploads\rbt\excel\new\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Artist Name English</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Rbt Name English</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Occasion</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>IVAS</t>
+  </si>
+  <si>
+    <t>Master Content Code</t>
   </si>
 </sst>
 </file>
@@ -153,16 +153,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +457,7 @@
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -482,45 +480,112 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
       </c>
       <c r="I2">
         <v>123</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>123</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>123</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>